<commit_message>
updated extract stock symbol and investment details functions. updated main() to change how spreadsheet is formatted
</commit_message>
<xml_diff>
--- a/data/reddit_posts.xlsx
+++ b/data/reddit_posts.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,1294 +464,911 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Only numbers that are correct about an option are its strike, expiry, and price. </t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AN</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>Buying Tesla Put</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$235 Put 11/1</t>
+        </is>
+      </c>
       <c r="D2" t="n">
-        <v>270</v>
+        <v>1525</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk4bc1/only_numbers_that_are_correct_about_an_option_are/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbq8fo/buying_tesla_put/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sell or Buy Options: Or both?</t>
+          <t>Strategy used by Tom Sosnoff - selling strangles 45DTE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>DTE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>44</v>
+        <v>543</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkbz8x/sell_or_buy_options_or_both/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbhk1h/strategy_used_by_tom_sosnoff_selling_strangles/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Advice on Hedging SPY.</t>
+          <t>$SPY moving sideways every afternoon...</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>6724</v>
+        <v>90</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkdcof/advice_on_hedging_spy/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbc6bk/spy_moving_sideways_every_afternoon/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Best Single Stock ETFs for Options</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>FOR</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Do far OTM options decrease in value faster than near-the-money ones? </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>628</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk11s7/best_single_stock_etfs_for_options/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbfvde/do_far_otm_options_decrease_in_value_faster_than/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Buying calls with a far out expiration date</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ARE</t>
-        </is>
-      </c>
+          <t>CPRI $40 puts were only $1 ?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>394</v>
+        <v>13364</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk3yw6/buying_calls_with_a_far_out_expiration_date/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbc6dz/cpri_40_puts_were_only_1/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tax implications of selling QQQ options versus letting them exercise to ETF</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>QQQ</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Does anyone trade a large number of contracts? 1,000+ at a time? </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>393</v>
+        <v>38680</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk91zq/tax_implications_of_selling_qqq_options_versus/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbwqbp/does_anyone_trade_a_large_number_of_contracts/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Box spread mark-to-market value and outlier/glitched price risks?</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>MARK</t>
-        </is>
-      </c>
+          <t>Earnings Played This Week - Beating The Market</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>2868</v>
+        <v>138352</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dknej0/box_spread_marktomarket_value_and_outlierglitched/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbdes6/earnings_played_this_week_beating_the_market/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Selling Covered Calls - Webull</t>
+          <t>Need Advice on Managing TSLA Call and Put Spreads!!! (I know I am stupid)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TYPE</t>
+          <t>TSLA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>5170</v>
+        <v>10</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkiah4/selling_covered_calls_webull/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbfiam/need_advice_on_managing_tsla_call_and_put_spreads/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A broker with low commisisons?</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
+          <t>Choosing high or low strike price?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>220</v>
+        <v>1395</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkhg19/a_broker_with_low_commisisons/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbvwyt/choosing_high_or_low_strike_price/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dell </t>
+          <t>RDDT CSP</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>DELL</t>
+          <t>CSP</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>15114</v>
+        <v>303</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkdfrx/dell/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbvfjl/rddt_csp/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Programming options buy/sell</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SEE</t>
-        </is>
-      </c>
+          <t>Synthetic Long Covered Naked Puts?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>107</v>
+        <v>14036</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkmkt9/programming_options_buysell/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbh96a/synthetic_long_covered_naked_puts/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Long Straddle vs. Long Call Calendar Spreads</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>CALL</t>
-        </is>
-      </c>
+          <t>Leaps</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>6050</v>
+        <v>17548</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkhtch/long_straddle_vs_long_call_calendar_spreads/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbfdmr/leaps/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Need Advice on Understanding PMCC Risk</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>Cash account limits</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>11980</v>
+        <v>12</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkhkb3/need_advice_on_understanding_pmcc_risk/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbefjy/cash_account_limits/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Robinhood flagged as a day trader</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Which of these is better? </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkmia2/robinhood_flagged_as_a_day_trader/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbt5u3/which_of_these_is_better/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Daily Discussion Thread for June 20, 2024</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>FOR</t>
-        </is>
-      </c>
+          <t>Can anyone relate to these fees</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>23619</v>
+        <v>3988</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dk84ni/daily_discussion_thread_for_june_20_2024/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbltoh/can_anyone_relate_to_these_fees/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>What Are Your Moves Tomorrow, June 21, 2024</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>ARE</t>
-        </is>
-      </c>
+          <t>Is possible to utilize excess liquidity?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>23619</v>
+        <v>26</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkky9f/what_are_your_moves_tomorrow_june_21_2024/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbwoey/is_possible_to_utilize_excess_liquidity/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Tesla merger?</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>ARE</t>
-        </is>
-      </c>
+          <t>Clarification of this trade setup</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>97</v>
+        <v>1442</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dk9pfd/tesla_merger/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbjhno/clarification_of_this_trade_setup/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>YOLO SQQQ Calls for Quad Witching!</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>QUAD</t>
-        </is>
-      </c>
+          <t>Basic knowledge</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkgc3n/yolo_sqqq_calls_for_quad_witching/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbw45m/basic_knowledge/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SMCI 1 week later</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SMCI</t>
-        </is>
-      </c>
+          <t>Selling low liquidity calls</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>31327</v>
+        <v>9</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkev19/smci_1_week_later/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbvh6n/selling_low_liquidity_calls/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>What are NVDA investors who are buying NVDA stock at 42 times revenues thinking?</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>AT</t>
-        </is>
-      </c>
+          <t>Any canadian here ?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>486</v>
+        <v>1185</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkjwd2/what_are_nvda_investors_who_are_buying_nvda_stock/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbe3wo/any_canadian_here/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Thought on $MMM? </t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Price jumps incommensurately at market open </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>630</v>
+        <v>24</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkb14f/thought_on_mmm/</t>
+          <t>https://www.reddit.com/r/options/comments/1gb7ppp/price_jumps_incommensurately_at_market_open/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Anyone hear of Nvidia and Uber owners robotics company SERV?</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>HEAR</t>
-        </is>
-      </c>
+          <t>Doubt</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>542</v>
+        <v>2</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkga8z/anyone_hear_of_nvidia_and_uber_owners_robotics/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbcdmq/doubt/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>$HOLO getting up this morning!!!</t>
+          <t>Doubt</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>4942</v>
+        <v>2</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbz86/holo_getting_up_this_morning/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbc5tg/doubt/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>HOLO - beginnings of a squeeze.</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>ALL</t>
-        </is>
-      </c>
+          <t>Turned $10k into $141k by inversing WSB (again)</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
-        <v>1711</v>
+        <v>16099</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkcj71/holo_beginnings_of_a_squeeze/</t>
+          <t>https://www.reddit.com/gallery/1gbcgva</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AEMD is low, buying more before it goes back up</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
+          <t xml:space="preserve">How is tsla q2 results not terrible? </t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
-        <v>444</v>
+        <v>3084</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkg1ge/aemd_is_low_buying_more_before_it_goes_back_up/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbq2ce/how_is_tsla_q2_results_not_terrible/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Trade Plan for June 20th!!!!!!!!</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>FOR</t>
-        </is>
-      </c>
+          <t>Intel announces plans for an investment of more than $28 billion for two new chip factories in Licking County, Ohio.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>909</v>
+        <v>1239</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkax0h/trade_plan_for_june_20th/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbukxe/intel_announces_plans_for_an_investment_of_more/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>What is the HOLO catalyst supposed to be?</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>AGO</t>
-        </is>
-      </c>
+          <t>Who thinks I can make this come back?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>4259</v>
+        <v>372</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkfjfz/what_is_the_holo_catalyst_supposed_to_be/</t>
+          <t>https://www.reddit.com/gallery/1gbrd0x</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ImmunityBio (IBRX) Announces Insurance Coverage of ANKTIVA</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
+          <t>what do i even do with myself</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>123</v>
+        <v>3800</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkctjm/immunitybio_ibrx_announces_insurance_coverage_of/</t>
+          <t>https://www.reddit.com/gallery/1gbiu0z</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tpst, trial results being released tomorrow </t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>What Are Your Moves Tomorrow, October 25, 2024</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>2171</v>
+        <v>41544</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dk2xey/tpst_trial_results_being_released_tomorrow/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbbs0c/what_are_your_moves_tomorrow_october_25_2024/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Why AEMD is flatlining despite short interest decreasing</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>AEMD</t>
-        </is>
-      </c>
+          <t>[NYSE official announcement: plans to extend U.S. stock trading hours to 22 hours a day]</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
-        <v>3421</v>
+        <v>513</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkcprw/why_aemd_is_flatlining_despite_short_interest/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbxvf2/nyse_official_announcement_plans_to_extend_us/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Why Sirius XM Holdings Inc (SIRI) is an Interesting Short Squeeze Opportunity</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>SIRI</t>
-        </is>
-      </c>
+          <t>Daily Discussion Thread for October 25, 2024</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>1469</v>
+        <v>41544</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dk85oj/why_sirius_xm_holdings_inc_siri_is_an_interesting/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbqlyo/daily_discussion_thread_for_october_25_2024/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>KTRA doing big things! Every, lets make some $$</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>BIG</t>
-        </is>
-      </c>
+          <t>Tesla earnings play</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="n">
-        <v>1529</v>
+        <v>305</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkk2el/ktra_doing_big_things_every_lets_make_some/</t>
+          <t>https://www.reddit.com/gallery/1gbgyv2</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">VHAI is popping and could be the next SOUN </t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>NEXT</t>
-        </is>
-      </c>
+          <t>Redwire - The 3rd Musketeer Rocketlab SpaceX</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
-        <v>5565</v>
+        <v>5572</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkjw0w/vhai_is_popping_and_could_be_the_next_soun/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gb9dbh/redwire_the_3rd_musketeer_rocketlab_spacex/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Can we have an ALLR discussion?</t>
+          <t xml:space="preserve">how is SBUX gaining while they’re business is still freefalling </t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>AN</t>
+          <t>SBUX</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
-        <v>78</v>
+        <v>19284</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dk95iz/can_we_have_an_allr_discussion/</t>
+          <t>https://www.reddit.com/gallery/1gboz55</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">VHAI has heavy potential and popping right now </t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>HAS</t>
-        </is>
-      </c>
+          <t>I own 100 shares of Tesla but...</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>5565</v>
+        <v>19</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dke0l6/vhai_has_heavy_potential_and_popping_right_now/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbja5f/i_own_100_shares_of_tesla_but/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>$PEGY Pineapple Subsidiary SUNation Surpasses Goal of $15 Million in Contracted Commercial Work</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
+          <t>10K loss in 5 months, I hate my life</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
-        <v>113</v>
+        <v>383</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkc85f/pegy_pineapple_subsidiary_sunation_surpasses_goal/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gb9aw9/10k_loss_in_5_months_i_hate_my_life/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Short Squeeze as AGBA/TRILLER $4 billion MERGER getting closer to completion...</t>
+          <t>$PCT Train Rides On - 2.7m Yolo Continues</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MOD</t>
+          <t>PCT</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="n">
-        <v>3170</v>
+        <v>3465</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkc7i9/short_squeeze_as_agbatriller_4_billion_merger/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbgwpl/pct_train_rides_on_27m_yolo_continues/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">$TELL thoughts? Looks like good entry point </t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
+          <t xml:space="preserve">This is by far my worst single trade this year. </t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
-        <v>4942</v>
+        <v>14591</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbuod/tell_thoughts_looks_like_good_entry_point/</t>
+          <t>https://www.reddit.com/gallery/1gbs8k1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>This looks like a bullish squeeze indicator to me. A sign of desperation?</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>AUTO</t>
-        </is>
-      </c>
+          <t xml:space="preserve">First time using margin. Easy money, buy my course. </t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkadll/this_looks_like_a_bullish_squeeze_indicator_to_me/</t>
+          <t>https://www.reddit.com/gallery/1gbgl1t</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Anyone holding mbio plz lmk asap ty</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>TY</t>
-        </is>
-      </c>
+          <t>New York Community Bank 3rd quarter loss</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="n">
-        <v>196</v>
+        <v>804</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkntp5/anyone_holding_mbio_plz_lmk_asap_ty/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbsajn/new_york_community_bank_3rd_quarter_loss/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DTC - Solid Value-Led Squeeze Setup</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>CASH</t>
-        </is>
-      </c>
+          <t>Anticipated earnings for next week.  Looking for the list</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
-        <v>4234</v>
+        <v>116</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkjxek/dtc_solid_valueled_squeeze_setup/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbxrcj/anticipated_earnings_for_next_week_looking_for/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Tpst , what happened there and why now?</t>
+          <t>(1985-2024) Nasdaq 100 (QQQ) vs 3x (TQQQ) and 5x (QQQ5) Leveraged. Calculated from NDX data from Yahoo Finance API.</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NOW</t>
+          <t>TQQQ</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="n">
-        <v>2171</v>
+        <v>3</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkicne/tpst_what_happened_there_and_why_now/</t>
+          <t>https://www.reddit.com/gallery/1gbezgw</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>AGBA/Triller $4bn Merger closing around the end of June... we're almost there. The Group files its Preliminary Proxy Statement</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>RE</t>
-        </is>
-      </c>
+          <t>The Edge in Calendar Spreads</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>3170</v>
+        <v>68</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkdk5o/agbatriller_4bn_merger_closing_around_the_end_of/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbi3wp/the_edge_in_calendar_spreads/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Can someone please explain what happened to $TPST</t>
+          <t>$IBRX  It's simple: A wee add, av down/up  =  Short Squeeze</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CAN</t>
+          <t>IBRX</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="n">
-        <v>62690</v>
+        <v>25701</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbs2a/can_someone_please_explain_what_happened_to_tpst/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbougi/ibrx_its_simple_a_wee_add_av_downup_short_squeeze/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>$AGBA/TRILLER $4 billion MERGER will be the Future...TikTok says US ban is inevitable without a court order blocking law</t>
+          <t xml:space="preserve">IBRX is skyrocketing this morning.  Was able to grab some shares right at opening.  Will get out when I think it’s still safe.  </t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="n">
-        <v>3170</v>
+        <v>21025</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dks0bl/agbatriller_4_billion_merger_will_be_the/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbuh7e/ibrx_is_skyrocketing_this_morning_was_able_to/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>$PBM crazy spike and then dip in AH worth a look imo</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>AH</t>
-        </is>
-      </c>
+          <t xml:space="preserve">FFIE is back!? 39% short and pumping in after hours. </t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
-        <v>157</v>
+        <v>3264</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkp1bl/pbm_crazy_spike_and_then_dip_in_ah_worth_a_look/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbqlrv/ffie_is_back_39_short_and_pumping_in_after_hours/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MPW massive potential…. This is the shorted stock..</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>MPW</t>
-        </is>
-      </c>
+          <t>SqueezeFinder - October 25th 2024</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
-        <v>631</v>
+        <v>2989</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkn9ho/mpw_massive_potential_this_is_the_shorted_stock/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbwneb/squeezefinder_october_25th_2024/</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Daily Discussion Thread</t>
+          <t>$ABVC smallcap bio penny with BIG potential and catalyst with huge recent news</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>ABVC</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
-        <v>77566</v>
+        <v>2094</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkkyvt/daily_discussion_thread/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbjdj1/abvc_smallcap_bio_penny_with_big_potential_and/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>$AIMD Ainos advances AI Nose tech in clinical trials...T.P. 4.25 (+300%)</t>
+          <t>$SLS  Do some DD this weekend, seriously. I'll get you started. Please add your comments below</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>SLS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="n">
-        <v>551</v>
+        <v>25701</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbeuy/aimd_ainos_advances_ai_nose_tech_in_clinical/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbyzju/sls_do_some_dd_this_weekend_seriously_ill_get_you/</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>MGOL is up like crazy all of a sudden again</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>ALL</t>
-        </is>
-      </c>
+          <t>I remember the HOLO YOLO trip to IBIZA guy</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
-        <v>1168</v>
+        <v>14447</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkaptk/mgol_is_up_like_crazy_all_of_a_sudden_again/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gby9m6/i_remember_the_holo_yolo_trip_to_ibiza_guy/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>$AGBA Merger is close and Shorts are going to get caught.</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>ARE</t>
-        </is>
-      </c>
+          <t>PBMWW HOWS EVERYONE DOING WITH THESE? OPPORTUNITY FOR MONEY.</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="n">
-        <v>1811</v>
+        <v>4585</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkadf5/agba_merger_is_close_and_shorts_are_going_to_get/</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>$CSSE any chance for a squeeze?</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>CSSE</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="n">
-        <v>7917</v>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkrqkj/csse_any_chance_for_a_squeeze/</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>$VLCN 300k total shares 1m market cap</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="n">
-        <v>3186</v>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkokr0/vlcn_300k_total_shares_1m_market_cap/</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Is no one looking at $SAVE? Looking ripe</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>AT</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="n">
-        <v>144</v>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkh8aw/is_no_one_looking_at_save_looking_ripe/</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>$MMA Can See Quick Jump Anytime</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>SEE</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="n">
-        <v>909</v>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkb01p/mma_can_see_quick_jump_anytime/</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Quick question for the group I was wondering </t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>FOR</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="n">
-        <v>165</v>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkaxks/quick_question_for_the_group_i_was_wondering/</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>TD Cowen Improves Ocular Therapeutix Stock on Clinical Advances</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>TD</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="n">
-        <v>551</v>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkapyt/td_cowen_improves_ocular_therapeutix_stock_on/</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>lmaoo would be sick if LPA starts hitting again, I have a couple shares that i got pretty low in that lol</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="n">
-        <v>4942</v>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkk5sw/lmaoo_would_be_sick_if_lpa_starts_hitting_again_i/</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>GOVXW went up 60000% today wtf??????</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="n">
-        <v>1168</v>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkhsjw/govxw_went_up_60000_today_wtf/</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>PLCE. Highest short interest stock that you you will find.</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>PLCE</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="n">
-        <v>4185</v>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkfv5a/plce_highest_short_interest_stock_that_you_you/</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>HOLO ain't looking too well right now</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>AIN</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="n">
-        <v>13132</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkdipe/holo_aint_looking_too_well_right_now/</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Did the ffie squeeze happen already? Or is there still a possibility?</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="n">
-        <v>7133</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbbe6/did_the_ffie_squeeze_happen_already_or_is_there/</t>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbl0ms/pbmww_hows_everyone_doing_with_these_opportunity/</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1383,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1804,1484 +1421,2010 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Box spread mark-to-market value and outlier/glitched price risks?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>MARK</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Does anyone trade a large number of contracts? 1,000+ at a time? </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>2868</v>
+        <v>38680</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dknej0/box_spread_marktomarket_value_and_outlierglitched/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbwqbp/does_anyone_trade_a_large_number_of_contracts/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Programming options buy/sell</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SEE</t>
-        </is>
-      </c>
+          <t>Is possible to utilize excess liquidity?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkmkt9/programming_options_buysell/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbwoey/is_possible_to_utilize_excess_liquidity/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Robinhood flagged as a day trader</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>Basic knowledge</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkmia2/robinhood_flagged_as_a_day_trader/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbw45m/basic_knowledge/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Selling Covered Calls - Webull</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>TYPE</t>
-        </is>
-      </c>
+          <t>Choosing high or low strike price?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>5170</v>
+        <v>1395</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkiah4/selling_covered_calls_webull/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbvwyt/choosing_high_or_low_strike_price/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Long Straddle vs. Long Call Calendar Spreads</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CALL</t>
-        </is>
-      </c>
+          <t>Selling low liquidity calls</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>6050</v>
+        <v>9</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkhtch/long_straddle_vs_long_call_calendar_spreads/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbvh6n/selling_low_liquidity_calls/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Need Advice on Understanding PMCC Risk</t>
+          <t>RDDT CSP</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>CSP</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>11980</v>
+        <v>303</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkhkb3/need_advice_on_understanding_pmcc_risk/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbvfjl/rddt_csp/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A broker with low commisisons?</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Which of these is better? </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>220</v>
+        <v>68</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkhg19/a_broker_with_low_commisisons/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbt5u3/which_of_these_is_better/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dell </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>DELL</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>Buying Tesla Put</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$235 Put 11/1</t>
+        </is>
+      </c>
       <c r="D9" t="n">
-        <v>15114</v>
+        <v>1525</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkdfrx/dell/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbq8fo/buying_tesla_put/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Advice on Hedging SPY.</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>Can anyone relate to these fees</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>6724</v>
+        <v>3988</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkdcof/advice_on_hedging_spy/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbltoh/can_anyone_relate_to_these_fees/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sell or Buy Options: Or both?</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>Clarification of this trade setup</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>44</v>
+        <v>1442</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dkbz8x/sell_or_buy_options_or_both/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbjhno/clarification_of_this_trade_setup/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tax implications of selling QQQ options versus letting them exercise to ETF</t>
+          <t>Strategy used by Tom Sosnoff - selling strangles 45DTE</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>QQQ</t>
+          <t>DTE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>393</v>
+        <v>543</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk91zq/tax_implications_of_selling_qqq_options_versus/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbhk1h/strategy_used_by_tom_sosnoff_selling_strangles/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Only numbers that are correct about an option are its strike, expiry, and price. </t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>AN</t>
-        </is>
-      </c>
+          <t>Synthetic Long Covered Naked Puts?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>270</v>
+        <v>14036</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk4bc1/only_numbers_that_are_correct_about_an_option_are/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbh96a/synthetic_long_covered_naked_puts/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Buying calls with a far out expiration date</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ARE</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Do far OTM options decrease in value faster than near-the-money ones? </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>394</v>
+        <v>628</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk3yw6/buying_calls_with_a_far_out_expiration_date/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbfvde/do_far_otm_options_decrease_in_value_faster_than/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Best Single Stock ETFs for Options</t>
+          <t>Need Advice on Managing TSLA Call and Put Spreads!!! (I know I am stupid)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>TSLA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/options/comments/1dk11s7/best_single_stock_etfs_for_options/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbfiam/need_advice_on_managing_tsla_call_and_put_spreads/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Screeners </t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
+          <t>Leaps</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>5105</v>
+        <v>17548</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkt6vf/screeners/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbfdmr/leaps/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ASTS? The Revenue Aspect Scares Me</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>LIVE</t>
-        </is>
-      </c>
+          <t>Cash account limits</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>-38</v>
+        <v>12</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkssfm/asts_the_revenue_aspect_scares_me/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbefjy/cash_account_limits/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Why the yesterday's selloff, my list</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>MY</t>
-        </is>
-      </c>
+          <t>Any canadian here ?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>7737</v>
+        <v>1185</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkr07s/why_the_yesterdays_selloff_my_list/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbe3wo/any_canadian_here/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>UNH Stock DD</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>UNH</t>
-        </is>
-      </c>
+          <t>Earnings Played This Week - Beating The Market</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>70</v>
+        <v>138352</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkpwgf/unh_stock_dd/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbdes6/earnings_played_this_week_beating_the_market/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Gilead GILD HIV prevention trial</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>GILD</t>
-        </is>
-      </c>
+          <t>Doubt</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>20534</v>
+        <v>2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkob03/gilead_gild_hiv_prevention_trial/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbcdmq/doubt/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">The future of AI is local </t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>AI</t>
-        </is>
-      </c>
+          <t>CPRI $40 puts were only $1 ?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>7753</v>
+        <v>13364</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dko3r9/the_future_of_ai_is_local/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbc6dz/cpri_40_puts_were_only_1/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Did I find an infinite money glitch?</t>
+          <t>$SPY moving sideways every afternoon...</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AN</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>2868</v>
+        <v>90</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkntt1/did_i_find_an_infinite_money_glitch/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbc6bk/spy_moving_sideways_every_afternoon/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>$NVDA Max Pain @83. Thoughts ?</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>NVDA</t>
-        </is>
-      </c>
+          <t>Doubt</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>8492</v>
+        <v>2</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkn87l/nvda_max_pain_83_thoughts/</t>
+          <t>https://www.reddit.com/r/options/comments/1gbc5tg/doubt/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">People who are playing stocks other than NVDA. Why? </t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>NVDA</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Price jumps incommensurately at market open </t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>2339</v>
+        <v>24</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkmny9/people_who_are_playing_stocks_other_than_nvda_why/</t>
+          <t>https://www.reddit.com/r/options/comments/1gb7ppp/price_jumps_incommensurately_at_market_open/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">My Thesis on IonQ
-</t>
+          <t>Is Elmo and his TSLA hurting you?</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>TSLA</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
-        <v>6250</v>
+        <v>581</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkmiva/my_thesis_on_ionq/</t>
+          <t>https://www.reddit.com/r/options/comments/1gb3o8w/is_elmo_and_his_tsla_hurting_you/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AAL</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>AAL</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Is it a known strategy to buy options at same strike w different expiration dates? </t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
-        <v>658</v>
+        <v>5179</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkm0lk/aal/</t>
+          <t>https://www.reddit.com/r/options/comments/1gb1sh1/is_it_a_known_strategy_to_buy_options_at_same/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SERV Robotics Partnered with NVIDIA and Uber</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>HAS</t>
-        </is>
-      </c>
+          <t>Is it possible to catch leftover limit orders from yesterday at open after a big price surge ?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>62</v>
+        <v>10817</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkldb6/serv_robotics_partnered_with_nvidia_and_uber/</t>
+          <t>https://www.reddit.com/r/options/comments/1gb1cdu/is_it_possible_to_catch_leftover_limit_orders/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>What Are Your Moves Tomorrow, June 21, 2024</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>ARE</t>
-        </is>
-      </c>
+          <t>Can you recommend a pro course? If such thing is even available</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>23619</v>
+        <v>9</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkky9f/what_are_your_moves_tomorrow_june_21_2024/</t>
+          <t>https://www.reddit.com/r/options/comments/1gb0anf/can_you_recommend_a_pro_course_if_such_thing_is/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>What are NVDA investors who are buying NVDA stock at 42 times revenues thinking?</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>AT</t>
-        </is>
-      </c>
+          <t>Seeking Ideas for Options Trading Tools and Software</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>486</v>
+        <v>49</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkjwd2/what_are_nvda_investors_who_are_buying_nvda_stock/</t>
+          <t>https://www.reddit.com/r/options/comments/1gazw9g/seeking_ideas_for_options_trading_tools_and/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>U | Unity Software Turnaround Incoming</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>BIG</t>
-        </is>
-      </c>
+          <t>Platform Reccomendations</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkjvi6/u_unity_software_turnaround_incoming/</t>
+          <t>https://www.reddit.com/r/options/comments/1gas1sv/platform_reccomendations/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NVDA is a value stock</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>NVDA</t>
-        </is>
-      </c>
+          <t>Beating The Market Using Double Debits &amp; PMCC's</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
-        <v>3741</v>
+        <v>138352</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkivg3/nvda_is_a_value_stock/</t>
+          <t>https://www.reddit.com/r/options/comments/1gaq7fz/beating_the_market_using_double_debits_pmccs/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Remember my call about the epic future tanking of $DJT?</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>MY</t>
-        </is>
-      </c>
+          <t>IWM and RUT Equivalence</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>22005</v>
+        <v>12220</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wallstreetbets/comments/1dkiph5/remember_my_call_about_the_epic_future_tanking_of/</t>
+          <t>https://www.reddit.com/r/options/comments/1gap9i5/iwm_and_rut_equivalence/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>$AGBA/TRILLER $4 billion MERGER will be the Future...TikTok says US ban is inevitable without a court order blocking law</t>
+          <t>Market Makers Messing Around</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="n">
-        <v>3170</v>
+        <v>3720</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dks0bl/agbatriller_4_billion_merger_will_be_the/</t>
+          <t>https://www.reddit.com/r/options/comments/1ganmsi/market_makers_messing_around/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>$CSSE any chance for a squeeze?</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>CSSE</t>
-        </is>
-      </c>
+          <t>Looking for a Swing Trading Signal App/Service with good success rate</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
-        <v>7917</v>
+        <v>2172</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkrqkj/csse_any_chance_for_a_squeeze/</t>
+          <t>https://www.reddit.com/r/options/comments/1gajrqq/looking_for_a_swing_trading_signal_appservice/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>$PBM crazy spike and then dip in AH worth a look imo</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>AH</t>
-        </is>
-      </c>
+          <t>SPX Debit Spreads…</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkp1bl/pbm_crazy_spike_and_then_dip_in_ah_worth_a_look/</t>
+          <t>https://www.reddit.com/r/options/comments/1gaifwh/spx_debit_spreads/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>$VLCN 300k total shares 1m market cap</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>CAP</t>
-        </is>
-      </c>
+          <t>Option Community</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>3186</v>
+        <v>42</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkokr0/vlcn_300k_total_shares_1m_market_cap/</t>
+          <t>https://www.reddit.com/r/options/comments/1gai54i/option_community/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Anyone holding mbio plz lmk asap ty</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>TY</t>
-        </is>
-      </c>
+          <t>Is there only one way to sell poor mans covered calls?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
-        <v>196</v>
+        <v>2327</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkntp5/anyone_holding_mbio_plz_lmk_asap_ty/</t>
+          <t>https://www.reddit.com/r/options/comments/1gai0ln/is_there_only_one_way_to_sell_poor_mans_covered/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MPW massive potential…. This is the shorted stock..</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>MPW</t>
-        </is>
-      </c>
+          <t>Bull Call Spread on McDonald's?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="n">
-        <v>631</v>
+        <v>5179</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkn9ho/mpw_massive_potential_this_is_the_shorted_stock/</t>
+          <t>https://www.reddit.com/r/options/comments/1gagbko/bull_call_spread_on_mcdonalds/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Daily Discussion Thread</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>Put/call ratio chart</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
-        <v>77566</v>
+        <v>74</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkkyvt/daily_discussion_thread/</t>
+          <t>https://www.reddit.com/r/options/comments/1gac07w/putcall_ratio_chart/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>lmaoo would be sick if LPA starts hitting again, I have a couple shares that i got pretty low in that lol</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
+          <t>Predicting Daily Volatility in SPY</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
-        <v>4942</v>
+        <v>5667</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkk5sw/lmaoo_would_be_sick_if_lpa_starts_hitting_again_i/</t>
+          <t>https://www.reddit.com/r/options/comments/1gabb8e/predicting_daily_volatility_in_spy/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>KTRA doing big things! Every, lets make some $$</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>BIG</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Course </t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="n">
-        <v>1529</v>
+        <v>5</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkk2el/ktra_doing_big_things_every_lets_make_some/</t>
+          <t>https://www.reddit.com/r/options/comments/1ga6fef/course/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DTC - Solid Value-Led Squeeze Setup</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>CASH</t>
-        </is>
-      </c>
+          <t>Warning to Options Traders: This Will Destroy You</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
-        <v>4234</v>
+        <v>2605</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkjxek/dtc_solid_valueled_squeeze_setup/</t>
+          <t>https://www.reddit.com/r/options/comments/1ga5wyu/warning_to_options_traders_this_will_destroy_you/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">VHAI is popping and could be the next SOUN </t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>NEXT</t>
-        </is>
-      </c>
+          <t>Nvda Call or put @143??</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="n">
-        <v>5565</v>
+        <v>9</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkjw0w/vhai_is_popping_and_could_be_the_next_soun/</t>
+          <t>https://www.reddit.com/r/options/comments/1ga4gk8/nvda_call_or_put_143/</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Tpst , what happened there and why now?</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>NOW</t>
-        </is>
-      </c>
+          <t>One sided wheel - covered calls for premiums?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>2171</v>
+        <v>179</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkicne/tpst_what_happened_there_and_why_now/</t>
+          <t>https://www.reddit.com/r/options/comments/1ga3fsk/one_sided_wheel_covered_calls_for_premiums/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GOVXW went up 60000% today wtf??????</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>Had an idea for selling SPY Options</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="n">
-        <v>1168</v>
+        <v>290</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkhsjw/govxw_went_up_60000_today_wtf/</t>
+          <t>https://www.reddit.com/r/options/comments/1ga32m0/had_an_idea_for_selling_spy_options/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Is no one looking at $SAVE? Looking ripe</t>
+          <t>CSP on SPY vs Buying SPY</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>CSP</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="n">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkh8aw/is_no_one_looking_at_save_looking_ripe/</t>
+          <t>https://www.reddit.com/r/options/comments/1ga2jbw/csp_on_spy_vs_buying_spy/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>AEMD is low, buying more before it goes back up</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
+          <t>reverse split</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
-        <v>444</v>
+        <v>5089</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkg1ge/aemd_is_low_buying_more_before_it_goes_back_up/</t>
+          <t>https://www.reddit.com/r/options/comments/1ga0kos/reverse_split/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PLCE. Highest short interest stock that you you will find.</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>PLCE</t>
-        </is>
-      </c>
+          <t>Selling naked call or buy put</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
-        <v>4185</v>
+        <v>348</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkfv5a/plce_highest_short_interest_stock_that_you_you/</t>
+          <t>https://www.reddit.com/r/options/comments/1g9zgcl/selling_naked_call_or_buy_put/</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>What is the HOLO catalyst supposed to be?</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>AGO</t>
-        </is>
-      </c>
+          <t>Is there any way I can get a complete list of weekly options?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
-        <v>4259</v>
+        <v>628</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkfjfz/what_is_the_holo_catalyst_supposed_to_be/</t>
+          <t>https://www.reddit.com/r/options/comments/1g9xbc2/is_there_any_way_i_can_get_a_complete_list_of/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t xml:space="preserve">VHAI has heavy potential and popping right now </t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>HAS</t>
-        </is>
-      </c>
+          <t>BABA has a clear share buyback strategy</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="n">
-        <v>5565</v>
+        <v>2</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dke0l6/vhai_has_heavy_potential_and_popping_right_now/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbzfpx/baba_has_a_clear_share_buyback_strategy/</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>AGBA/Triller $4bn Merger closing around the end of June... we're almost there. The Group files its Preliminary Proxy Statement</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>RE</t>
-        </is>
-      </c>
+          <t>The Hidden Truths About Trading Nobody Tells You: 4 Counter-Intuitive Facts</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
-        <v>3170</v>
+        <v>328</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkdk5o/agbatriller_4bn_merger_closing_around_the_end_of/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbyto6/the_hidden_truths_about_trading_nobody_tells_you/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>HOLO ain't looking too well right now</t>
+          <t>$KO</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>AIN</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="n">
-        <v>13132</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkdipe/holo_aint_looking_too_well_right_now/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbytkv/ko/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ImmunityBio (IBRX) Announces Insurance Coverage of ANKTIVA</t>
+          <t>Optimistic or pessimistic about $ON?</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>GOOD</t>
+          <t>ON</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="n">
-        <v>123</v>
+        <v>28</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkctjm/immunitybio_ibrx_announces_insurance_coverage_of/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbyr4v/optimistic_or_pessimistic_about_on/</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Why AEMD is flatlining despite short interest decreasing</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>AEMD</t>
-        </is>
-      </c>
+          <t>Is nobody able to explain how TF RKLB has risen so much more than LUNR and AST while riding on literally no news?</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="n">
-        <v>3421</v>
+        <v>33375</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkcprw/why_aemd_is_flatlining_despite_short_interest/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbycsn/is_nobody_able_to_explain_how_tf_rklb_has_risen/</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>HOLO - beginnings of a squeeze.</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>ALL</t>
-        </is>
-      </c>
+          <t>Shorting McDonald’s</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="n">
-        <v>1711</v>
+        <v>1180</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkcj71/holo_beginnings_of_a_squeeze/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbyand/shorting_mcdonalds/</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>$PEGY Pineapple Subsidiary SUNation Surpasses Goal of $15 Million in Contracted Commercial Work</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
+          <t>Undervalued ?</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="n">
-        <v>113</v>
+        <v>18</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkc85f/pegy_pineapple_subsidiary_sunation_surpasses_goal/</t>
+          <t>https://www.reddit.com/gallery/1gby3dt</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Short Squeeze as AGBA/TRILLER $4 billion MERGER getting closer to completion...</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>MOD</t>
-        </is>
-      </c>
+          <t>[NYSE official announcement: plans to extend U.S. stock trading hours to 22 hours a day]</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="n">
-        <v>3170</v>
+        <v>513</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkc7i9/short_squeeze_as_agbatriller_4_billion_merger/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbxvf2/nyse_official_announcement_plans_to_extend_us/</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>$HOLO getting up this morning!!!</t>
+          <t xml:space="preserve">Trump media mooners, where are you? </t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="n">
-        <v>4942</v>
+        <v>133</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbz86/holo_getting_up_this_morning/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbxu4f/trump_media_mooners_where_are_you/</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">$TELL thoughts? Looks like good entry point </t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
+          <t>Anticipated earnings for next week.  Looking for the list</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="n">
-        <v>4942</v>
+        <v>116</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbuod/tell_thoughts_looks_like_good_entry_point/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbxrcj/anticipated_earnings_for_next_week_looking_for/</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Can someone please explain what happened to $TPST</t>
+          <t>$JKS - Jinkosolar - China Solar Stocks Jump on Optimism Oversupply Will Be Addressed</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>CAN</t>
+          <t>JKS</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
-        <v>62690</v>
+        <v>3955</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbs2a/can_someone_please_explain_what_happened_to_tpst/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbwuzl/jks_jinkosolar_china_solar_stocks_jump_on/</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>$AIMD Ainos advances AI Nose tech in clinical trials...T.P. 4.25 (+300%)</t>
+          <t>I pulled out of Tesla after 3 years. Waiting to get back in $TSLA at a low price but terrified of missing another run up. What should I do?</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>AI</t>
+          <t>TSLA</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
-        <v>551</v>
+        <v>790</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbeuy/aimd_ainos_advances_ai_nose_tech_in_clinical/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbwocj/i_pulled_out_of_tesla_after_3_years_waiting_to/</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Did the ffie squeeze happen already? Or is there still a possibility?</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
+          <t>Rising Optimism: U.S. Consumer Sentiment Boosted by Income Hopes and Lower Rates</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="n">
-        <v>7133</v>
+        <v>11</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkbbe6/did_the_ffie_squeeze_happen_already_or_is_there/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbwelz/rising_optimism_us_consumer_sentiment_boosted_by/</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>$MMA Can See Quick Jump Anytime</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>SEE</t>
-        </is>
-      </c>
+          <t>NVIDIA Position with Inverse ETFs</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="n">
-        <v>909</v>
+        <v>-19</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkb01p/mma_can_see_quick_jump_anytime/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbunt4/nvidia_position_with_inverse_etfs/</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Quick question for the group I was wondering </t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>FOR</t>
-        </is>
-      </c>
+          <t>Intel announces plans for an investment of more than $28 billion for two new chip factories in Licking County, Ohio.</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="n">
-        <v>165</v>
+        <v>1239</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkaxks/quick_question_for_the_group_i_was_wondering/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbukxe/intel_announces_plans_for_an_investment_of_more/</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Trade Plan for June 20th!!!!!!!!</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>FOR</t>
-        </is>
-      </c>
+          <t>New York Community Bank 3rd quarter loss</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="n">
-        <v>909</v>
+        <v>804</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkax0h/trade_plan_for_june_20th/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbsajn/new_york_community_bank_3rd_quarter_loss/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>TD Cowen Improves Ocular Therapeutix Stock on Clinical Advances</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>TD</t>
-        </is>
-      </c>
+          <t xml:space="preserve">This is by far my worst single trade this year. </t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
-        <v>551</v>
+        <v>14591</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkapyt/td_cowen_improves_ocular_therapeutix_stock_on/</t>
+          <t>https://www.reddit.com/gallery/1gbs8k1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MGOL is up like crazy all of a sudden again</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>ALL</t>
-        </is>
-      </c>
+          <t>Who thinks I can make this come back?</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
-        <v>1168</v>
+        <v>372</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkaptk/mgol_is_up_like_crazy_all_of_a_sudden_again/</t>
+          <t>https://www.reddit.com/gallery/1gbrd0x</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>This looks like a bullish squeeze indicator to me. A sign of desperation?</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>AUTO</t>
-        </is>
-      </c>
+          <t>Daily Discussion Thread for October 25, 2024</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="n">
-        <v>634</v>
+        <v>41544</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkadll/this_looks_like_a_bullish_squeeze_indicator_to_me/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbqlyo/daily_discussion_thread_for_october_25_2024/</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>$AGBA Merger is close and Shorts are going to get caught.</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>ARE</t>
-        </is>
-      </c>
+          <t xml:space="preserve">How is tsla q2 results not terrible? </t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
-        <v>1811</v>
+        <v>3084</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dkadf5/agba_merger_is_close_and_shorts_are_going_to_get/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbq2ce/how_is_tsla_q2_results_not_terrible/</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Can we have an ALLR discussion?</t>
+          <t xml:space="preserve">how is SBUX gaining while they’re business is still freefalling </t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>AN</t>
+          <t>SBUX</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="n">
-        <v>78</v>
+        <v>19284</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dk95iz/can_we_have_an_allr_discussion/</t>
+          <t>https://www.reddit.com/gallery/1gboz55</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Why Sirius XM Holdings Inc (SIRI) is an Interesting Short Squeeze Opportunity</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>SIRI</t>
-        </is>
-      </c>
+          <t>I own 100 shares of Tesla but...</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="n">
-        <v>1469</v>
+        <v>19</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dk85oj/why_sirius_xm_holdings_inc_siri_is_an_interesting/</t>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbja5f/i_own_100_shares_of_tesla_but/</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tpst, trial results being released tomorrow </t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
+          <t>what do i even do with myself</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="n">
-        <v>2171</v>
+        <v>3800</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Shortsqueeze/comments/1dk2xey/tpst_trial_results_being_released_tomorrow/</t>
+          <t>https://www.reddit.com/gallery/1gbiu0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>market bias in the short sale?</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbilxp/market_bias_in_the_short_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Would You Consider NVDX a Safe Investment in an Unleveragd Portfolio?</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="n">
+        <v>-17</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/wallstreetbets/comments/1gbi93z/would_you_consider_nvdx_a_safe_investment_in_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>$SLS  Do some DD this weekend, seriously. I'll get you started. Please add your comments below</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>SLS</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="n">
+        <v>25701</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbyzju/sls_do_some_dd_this_weekend_seriously_ill_get_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>I remember the HOLO YOLO trip to IBIZA guy</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="n">
+        <v>14447</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gby9m6/i_remember_the_holo_yolo_trip_to_ibiza_guy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>SqueezeFinder - October 25th 2024</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="n">
+        <v>2989</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbwneb/squeezefinder_october_25th_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IBRX is skyrocketing this morning.  Was able to grab some shares right at opening.  Will get out when I think it’s still safe.  </t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="n">
+        <v>21025</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbuh7e/ibrx_is_skyrocketing_this_morning_was_able_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FFIE is back!? 39% short and pumping in after hours. </t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="n">
+        <v>3264</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbqlrv/ffie_is_back_39_short_and_pumping_in_after_hours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>$IBRX  It's simple: A wee add, av down/up  =  Short Squeeze</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>IBRX</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="n">
+        <v>25701</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbougi/ibrx_its_simple_a_wee_add_av_downup_short_squeeze/</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>PBMWW HOWS EVERYONE DOING WITH THESE? OPPORTUNITY FOR MONEY.</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="n">
+        <v>4585</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbl0ms/pbmww_hows_everyone_doing_with_these_opportunity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>$ABVC smallcap bio penny with BIG potential and catalyst with huge recent news</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ABVC</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="n">
+        <v>2094</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gbjdj1/abvc_smallcap_bio_penny_with_big_potential_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>SqueezeFinder - October 24th 2024</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="n">
+        <v>2989</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gb3lfe/squeezefinder_october_24th_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>I've been loading up on SGMO. One of the better microcap short squeeze candidates I see right now. Quick win on LRN, still holding WOLF, WVE, VERB</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>LRN</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="n">
+        <v>4286</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gatopw/ive_been_loading_up_on_sgmo_one_of_the_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>What about BJDX Bluejay Diagnostics - Big Increase in volume!!</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="n">
+        <v>422</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gajin8/what_about_bjdx_bluejay_diagnostics_big_increase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Check the volume on UAVS ! AgEagle. Yesterday was a good day for Archer and Joby !</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="n">
+        <v>21757</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gagyfo/check_the_volume_on_uavs_ageagle_yesterday_was_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>SCLX upcoming catalysts to consider</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="n">
+        <v>19785</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gacaut/sclx_upcoming_catalysts_to_consider/</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>SqueezeFinder - October 23rd 2024</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="n">
+        <v>2989</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gac0j5/squeezefinder_october_23rd_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>LRN short squeeze potential. Some dumbass Twitter short seller just got fucked</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>LRN</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="n">
+        <v>4286</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1gab823/lrn_short_squeeze_potential_some_dumbass_twitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>$SAVE let's talk about a real squeeze opportunity. High SI + Good News = Squeeze</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>SAVE</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="n">
+        <v>7281</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga8hhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>$NIXX heavily shorted; squeeze coming on 10/28; New company shares distribution in January 2025. Record date for shareholders 10/28</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>NIXX</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="n">
+        <v>844</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1ga6u1e/nixx_heavily_shorted_squeeze_coming_on_1028_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>You have stocks, I have an AI in need of training!</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="n">
+        <v>16352</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9y60v/you_have_stocks_i_have_an_ai_in_need_of_training/</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>$NIXX anticipated squeeze date 10/28</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NIXX</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="n">
+        <v>844</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9rrae/nixx_anticipated_squeeze_date_1028/</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$GRAB Broke resistance and held support today! </t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>GRAB</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="n">
+        <v>73260</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9rpgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$GRAB Broke resistance and held support today! </t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>GRAB</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="n">
+        <v>73260</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9rpah</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Under the Radar and at ATHs: $CMPO</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>CMPO</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="n">
+        <v>56558</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9qoat/under_the_radar_and_at_aths_cmpo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>🚨 EOSE Short Squeeze Potential 🚨</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="n">
+        <v>2461</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9pkn0/eose_short_squeeze_potential/</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$INUV alll Load up!! We going to make Shortsqueeze strong again! 🔥🔥🔥 </t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>INUV</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="n">
+        <v>378</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9o0wr/inuv_alll_load_up_we_going_to_make_shortsqueeze/</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Some $BBAI DD for you fellows. Also many other good plays in market ATM</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>BBAI</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="n">
+        <v>1985</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/SqueezePlays/comments/1g9eb4r/bbai_consolidating_and_covering_days_to_cover_has/</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Everybody is always looking for something earlyish. Look at the moves HOWL has made recently.</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="n">
+        <v>7469</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9l3l1/everybody_is_always_looking_for_something/</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$INUV All buy! Trying to see something… </t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>INUV</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="n">
+        <v>378</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9jags/inuv_all_buy_trying_to_see_something/</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$OCGN Below 1$ a bargain.  Their Eye tech worth Billions </t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>OCGN</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="n">
+        <v>25701</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g9g0wz/ocgn_below_1_a_bargain_their_eye_tech_worth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>$GRAB Breaking previous resistances 👀</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>GRAB</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="n">
+        <v>73260</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9apeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>$CAR - The Car Rental Short Squeeze (16% SI)</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>CAR</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="n">
+        <v>5222</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g97odn/car_the_car_rental_short_squeeze_16_si/</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are you watching PLUG MARA SOUN NIO RIOT (GEVO is flying wow) OPEN </t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>GEVO</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="n">
+        <v>21757</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g8ycfm/are_you_watching_plug_mara_soun_nio_riot_gevo_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>$ILLR Potential for Shortsqueeze is huge with Conor McGregor news.</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>ILLR</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="n">
+        <v>2009</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g8v090/illr_potential_for_shortsqueeze_is_huge_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>SqueezeFinder - October 21st 2024</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="n">
+        <v>2989</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g8tujh/squeezefinder_october_21st_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>PBMWW FROM THE GUY THAT CALLED ATER $3-20 PLCE 4-$19 BUY IT FOR 2 PENNYS!!</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="n">
+        <v>4585</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8tpu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>WULF(AI/Nuclear/BTC) Is anyone in this?</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="n">
+        <v>19467</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g8sg9y/wulfainuclearbtc_is_anyone_in_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$VSTM, Biopharma in dev stage </t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>VSTM</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="n">
+        <v>130</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g8rewy/vstm_biopharma_in_dev_stage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silversqueeze progression and sector internals  $$$  The train has left the station if you are going to get on board do it now.  </t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="n">
+        <v>28710</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Shortsqueeze/comments/1g8phgl/silversqueeze_progression_and_sector_internals/</t>
         </is>
       </c>
     </row>

</xml_diff>